<commit_message>
Included loose opportunistic points
</commit_message>
<xml_diff>
--- a/Sechelt_AOI/1_map_inputs/field_data/raw/Sechelt_FieldSampling_Aug2020.xlsx
+++ b/Sechelt_AOI/1_map_inputs/field_data/raw/Sechelt_FieldSampling_Aug2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\R\Sechelt_Cultural_Plants\Sechelt_AOI\1_map_inputs\field_data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\Sechelt_Cultural_Plants\Sechelt_AOI\1_map_inputs\field_data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{91C1AC2B-079C-4E09-8786-04F0A2D65470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41CBD79-13E6-48D5-B012-0A07380D78CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sechelt_site" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1337" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="306">
   <si>
     <t>Random</t>
   </si>
@@ -892,16 +892,67 @@
   </si>
   <si>
     <t>Op012_2020</t>
+  </si>
+  <si>
+    <t>Op032_2020</t>
+  </si>
+  <si>
+    <t>About 15 plants - haven't seen anywhere else</t>
+  </si>
+  <si>
+    <t>Op033_2020</t>
+  </si>
+  <si>
+    <t>Op034_2020</t>
+  </si>
+  <si>
+    <t>Op035_2020</t>
+  </si>
+  <si>
+    <t>Op036_2020</t>
+  </si>
+  <si>
+    <t>Op037_2020</t>
+  </si>
+  <si>
+    <t>Op038_2020</t>
+  </si>
+  <si>
+    <t>Op039_2020</t>
+  </si>
+  <si>
+    <t>Op040_2020</t>
+  </si>
+  <si>
+    <t>Op041_2020</t>
+  </si>
+  <si>
+    <t>Approx 10.6 cm dbh and 10 m tall</t>
+  </si>
+  <si>
+    <t>Approx 15.7 cm dbh and 12 m tall</t>
+  </si>
+  <si>
+    <t>Approx 32.0 cm dbh and 18 m tall</t>
+  </si>
+  <si>
+    <t>Approx 29.9 cm dbh, four individuals</t>
+  </si>
+  <si>
+    <t>Approx 13.7 cm dbh and 12m tall</t>
+  </si>
+  <si>
+    <t>Approx 14.8 cm dbh and 14m tall</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1032,6 +1083,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1387,7 +1444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1416,7 +1473,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1772,12 +1829,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7318,12 +7375,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9660,7 +9717,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>199</v>
       </c>
@@ -9677,7 +9734,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>199</v>
       </c>
@@ -9694,7 +9751,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>280</v>
       </c>
@@ -9714,7 +9771,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>280</v>
       </c>
@@ -9737,7 +9794,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>200</v>
       </c>
@@ -9760,7 +9817,199 @@
         <v>15</v>
       </c>
     </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>289</v>
+      </c>
+      <c r="B118">
+        <v>49.539870309999998</v>
+      </c>
+      <c r="C118">
+        <v>-123.8566486</v>
+      </c>
+      <c r="D118" t="s">
+        <v>97</v>
+      </c>
+      <c r="J118">
+        <v>0.5</v>
+      </c>
+      <c r="N118" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>291</v>
+      </c>
+      <c r="B119">
+        <v>49.539872299999999</v>
+      </c>
+      <c r="C119">
+        <v>-123.8566644</v>
+      </c>
+      <c r="D119" t="s">
+        <v>12</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>292</v>
+      </c>
+      <c r="B120">
+        <v>49.619656319999997</v>
+      </c>
+      <c r="C120">
+        <v>-123.9091349</v>
+      </c>
+      <c r="D120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G120">
+        <v>1</v>
+      </c>
+      <c r="N120" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>293</v>
+      </c>
+      <c r="B121">
+        <v>49.626260440000003</v>
+      </c>
+      <c r="C121">
+        <v>-123.91339480000001</v>
+      </c>
+      <c r="D121" t="s">
+        <v>268</v>
+      </c>
+      <c r="I121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>294</v>
+      </c>
+      <c r="B122">
+        <v>49.626505739999999</v>
+      </c>
+      <c r="C122">
+        <v>-123.9129263</v>
+      </c>
+      <c r="D122" t="s">
+        <v>268</v>
+      </c>
+      <c r="I122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>295</v>
+      </c>
+      <c r="B123">
+        <v>49.548385260000003</v>
+      </c>
+      <c r="C123">
+        <v>-123.8636647</v>
+      </c>
+      <c r="D123" t="s">
+        <v>38</v>
+      </c>
+      <c r="G123">
+        <v>1</v>
+      </c>
+      <c r="N123" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>296</v>
+      </c>
+      <c r="B124">
+        <v>49.539865839999997</v>
+      </c>
+      <c r="C124">
+        <v>-123.8566354</v>
+      </c>
+      <c r="D124" t="s">
+        <v>38</v>
+      </c>
+      <c r="H124">
+        <v>1</v>
+      </c>
+      <c r="N124" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>297</v>
+      </c>
+      <c r="B125">
+        <v>49.629460199999997</v>
+      </c>
+      <c r="C125">
+        <v>-123.9180411</v>
+      </c>
+      <c r="D125" t="s">
+        <v>60</v>
+      </c>
+      <c r="G125">
+        <v>1</v>
+      </c>
+      <c r="N125" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>298</v>
+      </c>
+      <c r="B126">
+        <v>49.628976979999997</v>
+      </c>
+      <c r="C126">
+        <v>-123.9177636</v>
+      </c>
+      <c r="D126" t="s">
+        <v>60</v>
+      </c>
+      <c r="G126">
+        <v>1</v>
+      </c>
+      <c r="N126" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>299</v>
+      </c>
+      <c r="B127">
+        <v>49.628381840000003</v>
+      </c>
+      <c r="C127">
+        <v>-123.91761049999999</v>
+      </c>
+      <c r="D127" t="s">
+        <v>60</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
+      <c r="N127" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>